<commit_message>
USD and JPY when Libor is not quoted
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/USD/USD_MainChecks.xlsx
+++ b/QuantLibXL/Data2/XLS/USD/USD_MainChecks.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sfondi\quantlib\QuantLibXL\Data2\XLS\USD\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="9585" yWindow="-15" windowWidth="9630" windowHeight="12015"/>
   </bookViews>
@@ -24,7 +19,7 @@
     <definedName name="TenYearsBondFutures">MainChecks!$C$4:$C$6</definedName>
     <definedName name="Trigger">MainChecks!$U$2</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -277,6 +272,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -805,6 +801,45 @@
 </styleSheet>
 </file>
 
+<file path=xl/volatileDependencies.xml><?xml version="1.0" encoding="utf-8"?>
+<volTypes xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <volType type="realTimeData">
+    <main first="pldatasource.rdatartdserver">
+      <tp t="s">
+        <v>Updated at 13:09:24</v>
+        <stp/>
+        <stp>{0FB3421B-4A46-427C-955B-8E68889990F0}</stp>
+        <tr r="Q5" s="2"/>
+      </tp>
+    </main>
+    <main first="pldatasource.rdatartdserver">
+      <tp t="s">
+        <v>Updated at 13:09:45</v>
+        <stp/>
+        <stp>{0B444CCA-A857-4BE7-9E7B-2B97C25198CB}</stp>
+        <tr r="P7" s="2"/>
+      </tp>
+    </main>
+    <main first="pldatasource.rdatartdserver">
+      <tp t="s">
+        <v>Updated at 13:09:08</v>
+        <stp/>
+        <stp>{EDEDFAC5-6600-405A-BE24-842457E52108}</stp>
+        <tr r="Q7" s="2"/>
+      </tp>
+    </main>
+    <main first="pldatasource.rdatartdserver">
+      <tp t="s">
+        <v>Updated at 13:09:08</v>
+        <stp/>
+        <stp>{FF7FCC8B-3666-4202-A2EC-99580E07E75B}</stp>
+        <tr r="Q6" s="2"/>
+      </tp>
+    </main>
+  </volType>
+</volTypes>
+</file>
+
 <file path=xl/activeX/activeX1.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{D7053240-CE69-11CD-A777-00DD01143C57}" ax:persistence="persistStreamInit" r:id="rId1"/>
 </file>
@@ -841,7 +876,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -849,20 +884,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:noFill/>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -896,7 +917,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -904,20 +925,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:noFill/>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -971,7 +978,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1006,7 +1013,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1246,7 +1253,8 @@
     <col min="19" max="19" width="2.7109375" style="2" customWidth="1"/>
     <col min="20" max="20" width="18.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="26.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="9.28515625" style="2"/>
+    <col min="22" max="36" width="9.28515625" style="2"/>
+    <col min="37" max="16384" width="9.28515625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="12" thickBot="1" x14ac:dyDescent="0.25">
@@ -1471,17 +1479,17 @@
         <v>TYcm1t</v>
       </c>
       <c r="L5" s="27">
-        <v>41992</v>
+        <v>42542</v>
       </c>
       <c r="M5" s="28">
-        <v>125.859375</v>
+        <v>129.921875</v>
       </c>
       <c r="N5" s="28"/>
       <c r="O5" s="28"/>
       <c r="P5" s="28"/>
-      <c r="Q5" s="29" t="e">
-        <f ca="1">_xll.RData(K5,{"EXPIR_DATE","LAST"},,"FRQ:1S",,L5)</f>
-        <v>#NAME?</v>
+      <c r="Q5" s="29" t="str">
+        <f>_xll.RData(K5,{"EXPIR_DATE","LAST"},,"FRQ:1S",,L5)</f>
+        <v>Updated at 13:09:24</v>
       </c>
       <c r="R5" s="8" t="s">
         <v>13</v>
@@ -1490,9 +1498,9 @@
       <c r="T5" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="U5" s="11" t="e">
-        <f ca="1">_xll.ohBoostVersion(Trigger)&amp;" / "&amp;_xll.ohVersion(Trigger)&amp;" / "&amp;_xll.qlVersion(Trigger)</f>
-        <v>#NAME?</v>
+      <c r="U5" s="11" t="str">
+        <f>_xll.ohBoostVersion(Trigger)&amp;" / "&amp;_xll.ohVersion(Trigger)&amp;" / "&amp;_xll.qlVersion(Trigger)</f>
+        <v>1_58 / 1.7.0 / 1.8</v>
       </c>
       <c r="V5" s="1"/>
       <c r="W5" s="1"/>
@@ -1537,22 +1545,22 @@
       </c>
       <c r="I6" s="3"/>
       <c r="J6" s="20"/>
-      <c r="K6" s="23" t="e">
-        <f ca="1">D14</f>
-        <v>#NAME?</v>
+      <c r="K6" s="23" t="str">
+        <f>D14</f>
+        <v>EDM6</v>
       </c>
       <c r="L6" s="24">
-        <v>42170</v>
+        <v>42534</v>
       </c>
       <c r="M6" s="30">
-        <v>99.5</v>
+        <v>99.320000000000007</v>
       </c>
       <c r="N6" s="30"/>
       <c r="O6" s="30"/>
       <c r="P6" s="30"/>
-      <c r="Q6" s="31" t="e">
-        <f ca="1">_xll.RData(K6,{"EXPIR_DATE","LAST"},,"FRQ:1S",,L6)</f>
-        <v>#NAME?</v>
+      <c r="Q6" s="31" t="str">
+        <f>_xll.RData(K6,{"EXPIR_DATE","LAST"},,"FRQ:1S",,L6)</f>
+        <v>Updated at 13:09:08</v>
       </c>
       <c r="R6" s="8" t="s">
         <v>13</v>
@@ -1561,9 +1569,9 @@
       <c r="T6" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="U6" s="11" t="e">
-        <f ca="1">_xll.ohRepositoryObjectCount(Trigger)</f>
-        <v>#NAME?</v>
+      <c r="U6" s="11">
+        <f>_xll.ohRepositoryObjectCount(Trigger)</f>
+        <v>1093</v>
       </c>
       <c r="V6" s="1"/>
       <c r="W6" s="1"/>
@@ -1613,25 +1621,25 @@
         <v>USDAM3L10Y</v>
       </c>
       <c r="L7" s="24">
-        <v>41919</v>
+        <v>42488</v>
       </c>
       <c r="M7" s="33" t="str">
         <f>N7&amp;"/"&amp;O7</f>
-        <v>2.497/2.527</v>
+        <v>1.67/1.71</v>
       </c>
       <c r="N7" s="30">
-        <v>2.4969999999999999</v>
+        <v>1.67</v>
       </c>
       <c r="O7" s="30">
-        <v>2.5270000000000001</v>
-      </c>
-      <c r="P7" s="30" t="e">
-        <f ca="1">_xll.RData(K7&amp;"="&amp;VLOOKUP(Currency,FuturesTable,7,0),{"BID","ASK"},,"FRQ:1S",,N7)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="Q7" s="31" t="e">
-        <f ca="1">_xll.RData(K7&amp;"="&amp;VLOOKUP(Currency,FuturesTable,7,0),"VALUE_DT1",,"FRQ:1S",,L7)</f>
-        <v>#NAME?</v>
+        <v>1.71</v>
+      </c>
+      <c r="P7" s="30" t="str">
+        <f>_xll.RData(K7&amp;"="&amp;VLOOKUP(Currency,FuturesTable,7,0),{"BID","ASK"},,"FRQ:1S",,N7)</f>
+        <v>Updated at 13:09:45</v>
+      </c>
+      <c r="Q7" s="31" t="str">
+        <f>_xll.RData(K7&amp;"="&amp;VLOOKUP(Currency,FuturesTable,7,0),"VALUE_DT1",,"FRQ:1S",,L7)</f>
+        <v>Updated at 13:09:08</v>
       </c>
       <c r="R7" s="8" t="s">
         <v>13</v>
@@ -1808,20 +1816,20 @@
         <f>PROPER(Currency)&amp;VLOOKUP(Currency,FuturesTable,8,0)&amp;VLOOKUP(Currency,FuturesTable,2,0)</f>
         <v>UsdLibor3M</v>
       </c>
-      <c r="L10" s="22" t="e">
-        <f ca="1">_xll.qlLastFixingQuoteReferenceDate(FirstIndex&amp;"LastFixing_Quote",Trigger)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="M10" s="32" t="e">
-        <f ca="1">_xll.qlQuoteValue(FirstIndex&amp;"LastFixing_Quote",Trigger)</f>
-        <v>#NAME?</v>
+      <c r="L10" s="22">
+        <f>_xll.qlLastFixingQuoteReferenceDate(FirstIndex&amp;"LastFixing_Quote",Trigger)</f>
+        <v>42488</v>
+      </c>
+      <c r="M10" s="32">
+        <f>_xll.qlQuoteValue(FirstIndex&amp;"LastFixing_Quote",Trigger)</f>
+        <v>6.3660000000000001E-3</v>
       </c>
       <c r="N10" s="32"/>
       <c r="O10" s="32"/>
       <c r="P10" s="32"/>
-      <c r="Q10" s="34" t="e">
-        <f ca="1">IF(AND(ISERROR(L10),ISERROR(M10)),_xll.ohRangeRetrieveError(L10)&amp;" "&amp;_xll.ohRangeRetrieveError(M10),IF(ISERROR(L10),_xll.ohRangeRetrieveError(L10),_xll.ohRangeRetrieveError(M10)))</f>
-        <v>#NAME?</v>
+      <c r="Q10" s="34" t="str">
+        <f>IF(AND(ISERROR(L10),ISERROR(M10)),_xll.ohRangeRetrieveError(L10)&amp;" "&amp;_xll.ohRangeRetrieveError(M10),IF(ISERROR(L10),_xll.ohRangeRetrieveError(L10),_xll.ohRangeRetrieveError(M10)))</f>
+        <v/>
       </c>
       <c r="R10" s="8" t="s">
         <v>13</v>
@@ -1876,20 +1884,20 @@
         <f>UPPER(Currency)&amp;"STD"</f>
         <v>USDSTD</v>
       </c>
-      <c r="L11" s="24" t="e">
-        <f ca="1">_xll.qlTermStructureReferenceDate(K11,Trigger)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="M11" s="25" t="e">
-        <f ca="1">_xll.qlYieldTSDiscount(K11,L11)</f>
-        <v>#NAME?</v>
+      <c r="L11" s="24">
+        <f>_xll.qlTermStructureReferenceDate(K11,Trigger)</f>
+        <v>42492</v>
+      </c>
+      <c r="M11" s="25">
+        <f>_xll.qlYieldTSDiscount(K11,L11)</f>
+        <v>1</v>
       </c>
       <c r="N11" s="25"/>
       <c r="O11" s="25"/>
       <c r="P11" s="25"/>
-      <c r="Q11" s="35" t="e">
-        <f ca="1">IF(ISERROR(L11),_xll.ohRangeRetrieveError(L11),_xll.ohRangeRetrieveError(M11))</f>
-        <v>#NAME?</v>
+      <c r="Q11" s="35" t="str">
+        <f>IF(ISERROR(L11),_xll.ohRangeRetrieveError(L11),_xll.ohRangeRetrieveError(M11))</f>
+        <v/>
       </c>
       <c r="R11" s="8" t="s">
         <v>13</v>
@@ -1938,20 +1946,20 @@
         <f>UPPER(Currency)&amp;"ON"</f>
         <v>USDON</v>
       </c>
-      <c r="L12" s="24" t="e">
-        <f ca="1">_xll.qlTermStructureReferenceDate(K12,Trigger)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="M12" s="25" t="e">
-        <f ca="1">_xll.qlYieldTSDiscount(K12,L12)</f>
-        <v>#NAME?</v>
+      <c r="L12" s="24">
+        <f>_xll.qlTermStructureReferenceDate(K12,Trigger)</f>
+        <v>42492</v>
+      </c>
+      <c r="M12" s="25">
+        <f>_xll.qlYieldTSDiscount(K12,L12)</f>
+        <v>1</v>
       </c>
       <c r="N12" s="25"/>
       <c r="O12" s="25"/>
       <c r="P12" s="25"/>
-      <c r="Q12" s="35" t="e">
-        <f ca="1">IF(ISERROR(L12),_xll.ohRangeRetrieveError(L12),_xll.ohRangeRetrieveError(M12))</f>
-        <v>#NAME?</v>
+      <c r="Q12" s="35" t="str">
+        <f>IF(ISERROR(L12),_xll.ohRangeRetrieveError(L12),_xll.ohRangeRetrieveError(M12))</f>
+        <v/>
       </c>
       <c r="R12" s="8" t="s">
         <v>13</v>
@@ -1990,20 +1998,20 @@
         <f>UPPER(Currency)&amp;"1M"</f>
         <v>USD1M</v>
       </c>
-      <c r="L13" s="24" t="e">
-        <f ca="1">_xll.qlTermStructureReferenceDate(K13,Trigger)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="M13" s="25" t="e">
-        <f ca="1">_xll.qlYieldTSDiscount(K13,L13)</f>
-        <v>#NAME?</v>
+      <c r="L13" s="24">
+        <f>_xll.qlTermStructureReferenceDate(K13,Trigger)</f>
+        <v>42494</v>
+      </c>
+      <c r="M13" s="25">
+        <f>_xll.qlYieldTSDiscount(K13,L13)</f>
+        <v>1</v>
       </c>
       <c r="N13" s="25"/>
       <c r="O13" s="25"/>
       <c r="P13" s="25"/>
-      <c r="Q13" s="36" t="e">
-        <f ca="1">IF(ISERROR(L13),_xll.ohRangeRetrieveError(L13),_xll.ohRangeRetrieveError(M13))</f>
-        <v>#NAME?</v>
+      <c r="Q13" s="36" t="str">
+        <f>IF(ISERROR(L13),_xll.ohRangeRetrieveError(L13),_xll.ohRangeRetrieveError(M13))</f>
+        <v/>
       </c>
       <c r="R13" s="8" t="s">
         <v>13</v>
@@ -2032,13 +2040,13 @@
       <c r="B14" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="C14" s="37" t="e">
-        <f t="array" aca="1" ref="C14:C17" ca="1">_xll.qlIMMNextDates(_xll.qlSettingsEvaluationDate(Trigger)-1,B14:B17)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="D14" s="6" t="e">
-        <f t="array" aca="1" ref="D14:D17" ca="1">VLOOKUP(Currency,FuturesTable,4,0)&amp;_xll.qlIMMcode(FuturesDates)</f>
-        <v>#NAME?</v>
+      <c r="C14" s="37">
+        <f t="array" ref="C14:C17">_xll.qlIMMNextDates(_xll.qlSettingsEvaluationDate(Trigger)-1,B14:B17)</f>
+        <v>42536</v>
+      </c>
+      <c r="D14" s="6" t="str">
+        <f t="array" ref="D14:D17">VLOOKUP(Currency,FuturesTable,4,0)&amp;_xll.qlIMMcode(FuturesDates)</f>
+        <v>EDM6</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
@@ -2050,20 +2058,20 @@
         <f>UPPER(Currency)&amp;"3M"</f>
         <v>USD3M</v>
       </c>
-      <c r="L14" s="24" t="e">
-        <f ca="1">_xll.qlTermStructureReferenceDate(K14,Trigger)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="M14" s="25" t="e">
-        <f ca="1">_xll.qlYieldTSDiscount(K14,L14)</f>
-        <v>#NAME?</v>
+      <c r="L14" s="24">
+        <f>_xll.qlTermStructureReferenceDate(K14,Trigger)</f>
+        <v>42494</v>
+      </c>
+      <c r="M14" s="25">
+        <f>_xll.qlYieldTSDiscount(K14,L14)</f>
+        <v>1</v>
       </c>
       <c r="N14" s="25"/>
       <c r="O14" s="25"/>
       <c r="P14" s="25"/>
-      <c r="Q14" s="36" t="e">
-        <f ca="1">IF(ISERROR(L14),_xll.ohRangeRetrieveError(L14),_xll.ohRangeRetrieveError(M14))</f>
-        <v>#NAME?</v>
+      <c r="Q14" s="36" t="str">
+        <f>IF(ISERROR(L14),_xll.ohRangeRetrieveError(L14),_xll.ohRangeRetrieveError(M14))</f>
+        <v/>
       </c>
       <c r="R14" s="8" t="s">
         <v>13</v>
@@ -2092,13 +2100,11 @@
       <c r="B15" s="40" t="b">
         <v>1</v>
       </c>
-      <c r="C15" s="38" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="D15" s="8" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+      <c r="C15" s="38">
+        <v>42634</v>
+      </c>
+      <c r="D15" s="8" t="str">
+        <v>EDU6</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
@@ -2110,20 +2116,20 @@
         <f>UPPER(Currency)&amp;"6M"</f>
         <v>USD6M</v>
       </c>
-      <c r="L15" s="24" t="e">
-        <f ca="1">_xll.qlTermStructureReferenceDate(K15,Trigger)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="M15" s="25" t="e">
-        <f ca="1">_xll.qlYieldTSDiscount(K15,L15)</f>
-        <v>#NAME?</v>
+      <c r="L15" s="24">
+        <f>_xll.qlTermStructureReferenceDate(K15,Trigger)</f>
+        <v>42494</v>
+      </c>
+      <c r="M15" s="25">
+        <f>_xll.qlYieldTSDiscount(K15,L15)</f>
+        <v>1</v>
       </c>
       <c r="N15" s="25"/>
       <c r="O15" s="25"/>
       <c r="P15" s="25"/>
-      <c r="Q15" s="36" t="e">
-        <f ca="1">IF(ISERROR(L15),_xll.ohRangeRetrieveError(L15),_xll.ohRangeRetrieveError(M15))</f>
-        <v>#NAME?</v>
+      <c r="Q15" s="36" t="str">
+        <f>IF(ISERROR(L15),_xll.ohRangeRetrieveError(L15),_xll.ohRangeRetrieveError(M15))</f>
+        <v/>
       </c>
       <c r="R15" s="8" t="s">
         <v>13</v>
@@ -2152,13 +2158,11 @@
       <c r="B16" s="40" t="b">
         <v>1</v>
       </c>
-      <c r="C16" s="38" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="D16" s="8" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+      <c r="C16" s="38">
+        <v>42725</v>
+      </c>
+      <c r="D16" s="8" t="str">
+        <v>EDZ6</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
@@ -2170,20 +2174,20 @@
         <f>UPPER(Currency)&amp;"1Y"</f>
         <v>USD1Y</v>
       </c>
-      <c r="L16" s="44" t="e">
-        <f ca="1">_xll.qlTermStructureReferenceDate(K16,Trigger)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="M16" s="45" t="e">
-        <f ca="1">_xll.qlYieldTSDiscount(K16,L16)</f>
-        <v>#NAME?</v>
+      <c r="L16" s="44">
+        <f>_xll.qlTermStructureReferenceDate(K16,Trigger)</f>
+        <v>42494</v>
+      </c>
+      <c r="M16" s="45">
+        <f>_xll.qlYieldTSDiscount(K16,L16)</f>
+        <v>1</v>
       </c>
       <c r="N16" s="45"/>
       <c r="O16" s="45"/>
       <c r="P16" s="45"/>
-      <c r="Q16" s="46" t="e">
-        <f ca="1">IF(ISERROR(L16),_xll.ohRangeRetrieveError(L16),_xll.ohRangeRetrieveError(M16))</f>
-        <v>#NAME?</v>
+      <c r="Q16" s="46" t="str">
+        <f>IF(ISERROR(L16),_xll.ohRangeRetrieveError(L16),_xll.ohRangeRetrieveError(M16))</f>
+        <v/>
       </c>
       <c r="R16" s="8" t="s">
         <v>13</v>
@@ -2212,13 +2216,11 @@
       <c r="B17" s="41" t="b">
         <v>1</v>
       </c>
-      <c r="C17" s="39" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="D17" s="10" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+      <c r="C17" s="39">
+        <v>42809</v>
+      </c>
+      <c r="D17" s="10" t="str">
+        <v>EDH7</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
@@ -5409,17 +5411,72 @@
       <c r="AI100" s="3"/>
       <c r="AJ100" s="3"/>
     </row>
-    <row r="101" spans="1:36" s="47" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="102" spans="1:36" s="47" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="J102" s="2"/>
-      <c r="K102" s="2"/>
-      <c r="L102" s="2"/>
-      <c r="M102" s="2"/>
-      <c r="N102" s="2"/>
-      <c r="O102" s="2"/>
-      <c r="P102" s="2"/>
-      <c r="Q102" s="2"/>
-      <c r="R102" s="2"/>
+    <row r="101" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A101" s="47"/>
+      <c r="B101" s="47"/>
+      <c r="C101" s="47"/>
+      <c r="D101" s="47"/>
+      <c r="E101" s="47"/>
+      <c r="F101" s="47"/>
+      <c r="G101" s="47"/>
+      <c r="H101" s="47"/>
+      <c r="I101" s="47"/>
+      <c r="J101" s="47"/>
+      <c r="K101" s="47"/>
+      <c r="L101" s="47"/>
+      <c r="M101" s="47"/>
+      <c r="N101" s="47"/>
+      <c r="O101" s="47"/>
+      <c r="P101" s="47"/>
+      <c r="Q101" s="47"/>
+      <c r="R101" s="47"/>
+      <c r="S101" s="47"/>
+      <c r="T101" s="47"/>
+      <c r="U101" s="47"/>
+      <c r="V101" s="47"/>
+      <c r="W101" s="47"/>
+      <c r="X101" s="47"/>
+      <c r="Y101" s="47"/>
+      <c r="Z101" s="47"/>
+      <c r="AA101" s="47"/>
+      <c r="AB101" s="47"/>
+      <c r="AC101" s="47"/>
+      <c r="AD101" s="47"/>
+      <c r="AE101" s="47"/>
+      <c r="AF101" s="47"/>
+      <c r="AG101" s="47"/>
+      <c r="AH101" s="47"/>
+      <c r="AI101" s="47"/>
+      <c r="AJ101" s="47"/>
+    </row>
+    <row r="102" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A102" s="47"/>
+      <c r="B102" s="47"/>
+      <c r="C102" s="47"/>
+      <c r="D102" s="47"/>
+      <c r="E102" s="47"/>
+      <c r="F102" s="47"/>
+      <c r="G102" s="47"/>
+      <c r="H102" s="47"/>
+      <c r="I102" s="47"/>
+      <c r="S102" s="47"/>
+      <c r="T102" s="47"/>
+      <c r="U102" s="47"/>
+      <c r="V102" s="47"/>
+      <c r="W102" s="47"/>
+      <c r="X102" s="47"/>
+      <c r="Y102" s="47"/>
+      <c r="Z102" s="47"/>
+      <c r="AA102" s="47"/>
+      <c r="AB102" s="47"/>
+      <c r="AC102" s="47"/>
+      <c r="AD102" s="47"/>
+      <c r="AE102" s="47"/>
+      <c r="AF102" s="47"/>
+      <c r="AG102" s="47"/>
+      <c r="AH102" s="47"/>
+      <c r="AI102" s="47"/>
+      <c r="AJ102" s="47"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -5436,7 +5493,7 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1026" r:id="rId4" name="CommandButton2">
+        <control shapeId="1025" r:id="rId4" name="CommandButton1">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
@@ -5456,12 +5513,12 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1026" r:id="rId4" name="CommandButton2"/>
+        <control shapeId="1025" r:id="rId4" name="CommandButton1"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId6" name="CommandButton1">
+        <control shapeId="1026" r:id="rId6" name="CommandButton2">
           <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
@@ -5481,7 +5538,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1025" r:id="rId6" name="CommandButton1"/>
+        <control shapeId="1026" r:id="rId6" name="CommandButton2"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>